<commit_message>
Updated Gantt Chart save file
</commit_message>
<xml_diff>
--- a/Documents/Gantt Chart.xlsx
+++ b/Documents/Gantt Chart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\OneDrive\Desktop\Projects\FMCW Radar Simulation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\OneDrive\Desktop\Projects\FMCW Radar Simulation\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A828F33-5DA2-416D-BA3C-5F6F347EFE80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42FFEE5-71C9-45EB-B31E-7174A8AB667E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{B79F7859-B868-468E-BFBE-84DA97D1A561}"/>
   </bookViews>
@@ -87,7 +87,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -106,8 +106,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4EA72E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -161,21 +167,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -254,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -279,7 +270,7 @@
     <xf numFmtId="16" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -291,13 +282,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -306,6 +303,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF4EA72E"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -637,7 +639,7 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -654,37 +656,37 @@
         <v>46000</v>
       </c>
       <c r="C1" s="9">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="D1" s="9">
-        <v>46004</v>
+        <v>46006</v>
       </c>
       <c r="E1" s="9">
-        <v>46006</v>
+        <v>46009</v>
       </c>
       <c r="F1" s="9">
-        <v>46008</v>
+        <v>46012</v>
       </c>
       <c r="G1" s="9">
-        <v>46010</v>
+        <v>46015</v>
       </c>
       <c r="H1" s="9">
-        <v>46012</v>
+        <v>46018</v>
       </c>
       <c r="I1" s="9">
-        <v>46014</v>
+        <v>46021</v>
       </c>
       <c r="J1" s="9">
-        <v>46016</v>
+        <v>46024</v>
       </c>
       <c r="K1" s="9">
-        <v>46018</v>
+        <v>46027</v>
       </c>
       <c r="L1" s="9">
-        <v>46020</v>
-      </c>
-      <c r="M1" s="10">
-        <v>46022</v>
+        <v>46030</v>
+      </c>
+      <c r="M1" s="9">
+        <v>46033</v>
       </c>
       <c r="O1" s="2"/>
       <c r="P1" s="1" t="s">
@@ -692,7 +694,7 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5"/>
@@ -706,31 +708,31 @@
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
-      <c r="M2" s="12"/>
+      <c r="M2" s="11"/>
       <c r="O2" s="3"/>
       <c r="P2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="6"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="17"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
-      <c r="M3" s="12"/>
+      <c r="M3" s="11"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="4"/>
@@ -738,30 +740,30 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="4"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="16"/>
       <c r="L4" s="4"/>
-      <c r="M4" s="12"/>
+      <c r="M4" s="11"/>
     </row>
     <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="16"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>